<commit_message>
add all data into excel
</commit_message>
<xml_diff>
--- a/all data of average stay.xlsx
+++ b/all data of average stay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Anaconda3\envs\MachineLearning2\TrafficSignalDRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB0DBC3-679B-494B-ABA3-2E8E5118B33C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A673954-67B3-4644-8892-1E0C4CA2CC16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9F3547D9-27BD-4565-AF91-85CC7D87BDD8}"/>
   </bookViews>
@@ -25,6 +25,16 @@
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">[1]Sheet!$A$31</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">[1]Sheet!$A$32</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">[1]Sheet!$A$33</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">[1]Sheet!$A$34</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">[1]Sheet!$B$31:$V$31</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">[1]Sheet!$B$32:$V$32</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">[1]Sheet!$B$33:$V$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">[1]Sheet!$B$34:$V$34</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="39">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -157,6 +167,10 @@
     <t>std</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>avg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -237,18 +251,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet!$A$31</c:f>
+              <c:f>工作表1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -257,17 +272,81 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$B$2:$V$2</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>t0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>t1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>t2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>t3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>t4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>t5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>t6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>t7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>t10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>t11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>t12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>t13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>t14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>t15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>t16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>t17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>t18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>t19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>t20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet!$B$31:$V$31</c:f>
+              <c:f>工作表1!$B$3:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -337,10 +416,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E667-49F5-8915-978938B91399}"/>
+              <c16:uniqueId val="{00000000-E0AA-4849-8261-D1C6C5F11CF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -349,7 +427,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet!$A$32</c:f>
+              <c:f>工作表1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -358,17 +436,81 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$B$2:$V$2</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>t0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>t1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>t2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>t3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>t4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>t5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>t6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>t7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>t10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>t11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>t12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>t13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>t14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>t15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>t16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>t17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>t18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>t19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>t20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet!$B$32:$V$32</c:f>
+              <c:f>工作表1!$B$4:$V$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -438,10 +580,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E667-49F5-8915-978938B91399}"/>
+              <c16:uniqueId val="{00000001-E0AA-4849-8261-D1C6C5F11CF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -450,7 +591,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet!$A$33</c:f>
+              <c:f>工作表1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -459,17 +600,81 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$B$2:$V$2</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>t0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>t1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>t2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>t3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>t4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>t5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>t6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>t7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>t10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>t11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>t12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>t13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>t14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>t15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>t16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>t17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>t18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>t19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>t20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet!$B$33:$V$33</c:f>
+              <c:f>工作表1!$B$5:$V$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -539,10 +744,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E667-49F5-8915-978938B91399}"/>
+              <c16:uniqueId val="{00000002-E0AA-4849-8261-D1C6C5F11CF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -551,7 +755,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet!$A$34</c:f>
+              <c:f>工作表1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -560,17 +764,81 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$B$2:$V$2</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>t0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>t1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>t2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>t3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>t4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>t5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>t6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>t7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>t8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>t9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>t10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>t11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>t12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>t13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>t14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>t15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>t16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>t17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>t18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>t19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>t20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet!$B$34:$V$34</c:f>
+              <c:f>工作表1!$B$6:$V$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -640,10 +908,9 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E667-49F5-8915-978938B91399}"/>
+              <c16:uniqueId val="{00000003-E0AA-4849-8261-D1C6C5F11CF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -655,29 +922,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="10"/>
-        <c:axId val="100"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="1795284351"/>
+        <c:axId val="1795281023"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="10"/>
+        <c:axId val="1795284351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100"/>
+        <c:crossAx val="1795281023"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100"/>
+        <c:axId val="1795281023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,10 +953,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10"/>
+        <c:crossAx val="1795284351"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -699,12 +967,19 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -5652,7 +5927,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>290286</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5685,9 +5960,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>328839</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5717,10 +5992,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>208643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5750,10 +6025,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>526142</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>72571</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5783,10 +6058,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5816,10 +6091,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5849,10 +6124,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>226786</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>154215</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -5882,10 +6157,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400000" cy="2700000"/>
     <xdr:graphicFrame macro="">
@@ -6213,249 +6488,6 @@
         <row r="31">
           <cell r="B31">
             <v>97.005636070853498</v>
-          </cell>
-          <cell r="C31">
-            <v>162.07058823529411</v>
-          </cell>
-          <cell r="D31">
-            <v>132.4489695780178</v>
-          </cell>
-          <cell r="E31">
-            <v>105.8647595356552</v>
-          </cell>
-          <cell r="F31">
-            <v>92.64072000000013</v>
-          </cell>
-          <cell r="G31">
-            <v>85.837846153846044</v>
-          </cell>
-          <cell r="H31">
-            <v>98.521452145214568</v>
-          </cell>
-          <cell r="I31">
-            <v>106.8099829351535</v>
-          </cell>
-          <cell r="J31">
-            <v>107.61457800511501</v>
-          </cell>
-          <cell r="K31">
-            <v>101.0956125827815</v>
-          </cell>
-          <cell r="L31">
-            <v>140.16631111111101</v>
-          </cell>
-          <cell r="M31">
-            <v>121.5986891385766</v>
-          </cell>
-          <cell r="N31">
-            <v>117.4368049426303</v>
-          </cell>
-          <cell r="O31">
-            <v>157.33980322003589</v>
-          </cell>
-          <cell r="P31">
-            <v>103.5562969140951</v>
-          </cell>
-          <cell r="Q31">
-            <v>157.30922587486739</v>
-          </cell>
-          <cell r="R31">
-            <v>116.1640569395018</v>
-          </cell>
-          <cell r="S31">
-            <v>98.060080645161406</v>
-          </cell>
-          <cell r="T31">
-            <v>100.7225043782836</v>
-          </cell>
-          <cell r="U31">
-            <v>88.27986003110432</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>94.81782642689609</v>
-          </cell>
-          <cell r="C32">
-            <v>148.8977225672877</v>
-          </cell>
-          <cell r="D32">
-            <v>135.4080291970802</v>
-          </cell>
-          <cell r="E32">
-            <v>102.5194331983806</v>
-          </cell>
-          <cell r="F32">
-            <v>92.156344772545793</v>
-          </cell>
-          <cell r="G32">
-            <v>82.254433307633093</v>
-          </cell>
-          <cell r="H32">
-            <v>85.490996015936204</v>
-          </cell>
-          <cell r="I32">
-            <v>114.2332456140349</v>
-          </cell>
-          <cell r="J32">
-            <v>106.931881676253</v>
-          </cell>
-          <cell r="K32">
-            <v>89.012702265372084</v>
-          </cell>
-          <cell r="L32">
-            <v>127.9519616390584</v>
-          </cell>
-          <cell r="M32">
-            <v>147.31997950819661</v>
-          </cell>
-          <cell r="N32">
-            <v>113.1532244196045</v>
-          </cell>
-          <cell r="O32">
-            <v>151.3667584940311</v>
-          </cell>
-          <cell r="P32">
-            <v>109.5097381342062</v>
-          </cell>
-          <cell r="Q32">
-            <v>154.7632172131145</v>
-          </cell>
-          <cell r="R32">
-            <v>136.34077212806011</v>
-          </cell>
-          <cell r="S32">
-            <v>95.159046052631325</v>
-          </cell>
-          <cell r="T32">
-            <v>88.983411949685774</v>
-          </cell>
-          <cell r="U32">
-            <v>96.152405063291212</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>97.029026845637503</v>
-          </cell>
-          <cell r="C33">
-            <v>134.03036597428269</v>
-          </cell>
-          <cell r="D33">
-            <v>137.97205607476641</v>
-          </cell>
-          <cell r="E33">
-            <v>112.0877673224979</v>
-          </cell>
-          <cell r="F33">
-            <v>90.432947530864155</v>
-          </cell>
-          <cell r="G33">
-            <v>82.753003802281285</v>
-          </cell>
-          <cell r="H33">
-            <v>92.279132569557959</v>
-          </cell>
-          <cell r="I33">
-            <v>123.4468141592918</v>
-          </cell>
-          <cell r="J33">
-            <v>103.229008264463</v>
-          </cell>
-          <cell r="K33">
-            <v>99.912155172413932</v>
-          </cell>
-          <cell r="L33">
-            <v>125.5179930795848</v>
-          </cell>
-          <cell r="M33">
-            <v>138.05768463073861</v>
-          </cell>
-          <cell r="N33">
-            <v>119.96755447941889</v>
-          </cell>
-          <cell r="O33">
-            <v>158.1629870129872</v>
-          </cell>
-          <cell r="P33">
-            <v>110.14434857635889</v>
-          </cell>
-          <cell r="Q33">
-            <v>167.4501096491226</v>
-          </cell>
-          <cell r="R33">
-            <v>137.90425531914869</v>
-          </cell>
-          <cell r="S33">
-            <v>102.2127241673783</v>
-          </cell>
-          <cell r="T33">
-            <v>90.936392156863008</v>
-          </cell>
-          <cell r="U33">
-            <v>95.188467741935582</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>89.720356037151561</v>
-          </cell>
-          <cell r="C34">
-            <v>155.4008869179595</v>
-          </cell>
-          <cell r="D34">
-            <v>152.42381852551941</v>
-          </cell>
-          <cell r="E34">
-            <v>102.7958609271524</v>
-          </cell>
-          <cell r="F34">
-            <v>91.452791068580453</v>
-          </cell>
-          <cell r="G34">
-            <v>84.090629921259776</v>
-          </cell>
-          <cell r="H34">
-            <v>110.1553633217994</v>
-          </cell>
-          <cell r="I34">
-            <v>115.34311688311681</v>
-          </cell>
-          <cell r="J34">
-            <v>101.24873675631621</v>
-          </cell>
-          <cell r="K34">
-            <v>103.1494779116465</v>
-          </cell>
-          <cell r="L34">
-            <v>117.0527586206895</v>
-          </cell>
-          <cell r="M34">
-            <v>140.0303999999999</v>
-          </cell>
-          <cell r="N34">
-            <v>111.4933501683502</v>
-          </cell>
-          <cell r="O34">
-            <v>155.10229681978791</v>
-          </cell>
-          <cell r="P34">
-            <v>87.278841512469782</v>
-          </cell>
-          <cell r="Q34">
-            <v>166.28076923076949</v>
-          </cell>
-          <cell r="R34">
-            <v>116.0634189548271</v>
-          </cell>
-          <cell r="S34">
-            <v>98.143324937027785</v>
-          </cell>
-          <cell r="T34">
-            <v>88.844677544677467</v>
-          </cell>
-          <cell r="U34">
-            <v>112.3150136487716</v>
           </cell>
         </row>
         <row r="59">
@@ -9837,15 +9869,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320D79F4-73EA-4B77-A7FB-1589FAB87756}">
-  <dimension ref="A1:X108"/>
+  <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X86" sqref="X86"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -9853,7 +9889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -9923,8 +9959,11 @@
       <c r="X2" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="Y2" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -9995,8 +10034,12 @@
         <f>_xlfn.STDEV.S(B3:V3)</f>
         <v>13.199486504106654</v>
       </c>
+      <c r="Y3">
+        <f>AVERAGE(,B3:V3)</f>
+        <v>37.716113135643816</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -10067,8 +10110,12 @@
         <f>_xlfn.STDEV.S(B4:V4)</f>
         <v>12.702645015492015</v>
       </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y6" si="0">AVERAGE(,B4:V4)</f>
+        <v>38.381010830991443</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -10136,11 +10183,15 @@
         <v>32.211130167780702</v>
       </c>
       <c r="X5">
-        <f t="shared" ref="X5:X68" si="0">_xlfn.STDEV.S(B5:V5)</f>
+        <f t="shared" ref="X5:X61" si="1">_xlfn.STDEV.S(B5:V5)</f>
         <v>9.1119735844290162</v>
       </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>34.987004082651531</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -10208,11 +10259,15 @@
         <v>65.897747728472268</v>
       </c>
       <c r="X6">
+        <f t="shared" si="1"/>
+        <v>4.2242079181595251</v>
+      </c>
+      <c r="Y6">
         <f t="shared" si="0"/>
-        <v>4.2242079181595251</v>
+        <v>62.973696592468293</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -10220,7 +10275,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -10290,8 +10345,11 @@
       <c r="X15" t="s">
         <v>36</v>
       </c>
+      <c r="Y15" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -10359,11 +10417,15 @@
         <v>105.8560809217749</v>
       </c>
       <c r="X16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.596668987281088</v>
       </c>
+      <c r="Y16">
+        <f t="shared" ref="Y16:Y23" si="2">AVERAGE(,B16:V16)</f>
+        <v>112.29374297921805</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -10431,11 +10493,15 @@
         <v>96.023937235472275</v>
       </c>
       <c r="X17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.269710519508006</v>
       </c>
+      <c r="Y17">
+        <f t="shared" si="2"/>
+        <v>113.71606183172007</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -10503,11 +10569,15 @@
         <v>83.261641061386541</v>
       </c>
       <c r="X18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.744426274009662</v>
       </c>
+      <c r="Y18">
+        <f t="shared" si="2"/>
+        <v>106.89452802617751</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -10575,11 +10645,15 @@
         <v>103.4073697510468</v>
       </c>
       <c r="X19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.078652930786642</v>
       </c>
+      <c r="Y19">
+        <f t="shared" si="2"/>
+        <v>109.74503596506082</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -10647,11 +10721,15 @@
         <v>95.693805643769764</v>
       </c>
       <c r="X20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.549480643977208</v>
       </c>
+      <c r="Y20">
+        <f t="shared" si="2"/>
+        <v>110.7697120849119</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -10719,11 +10797,15 @@
         <v>89.662639712853348</v>
       </c>
       <c r="X21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.817712932016377</v>
       </c>
+      <c r="Y21">
+        <f t="shared" si="2"/>
+        <v>106.19722866897017</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -10791,11 +10873,15 @@
         <v>97.609201363025448</v>
       </c>
       <c r="X22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.08814587405789</v>
       </c>
+      <c r="Y22">
+        <f t="shared" si="2"/>
+        <v>108.25906946137746</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -10863,11 +10949,15 @@
         <v>109.76734230232709</v>
       </c>
       <c r="X23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.251175230394345</v>
       </c>
+      <c r="Y23">
+        <f t="shared" si="2"/>
+        <v>112.34344472531558</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -10875,7 +10965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -10945,8 +11035,11 @@
       <c r="X29" t="s">
         <v>36</v>
       </c>
+      <c r="Y29" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -11014,11 +11107,15 @@
         <v>28.488281582175389</v>
       </c>
       <c r="X30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.370938541377406</v>
       </c>
+      <c r="Y30">
+        <f t="shared" ref="Y30:Y33" si="3">AVERAGE(,B30:V30)</f>
+        <v>32.290944093923947</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -11086,11 +11183,15 @@
         <v>27.113861944363471</v>
       </c>
       <c r="X31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.046623009607959</v>
       </c>
+      <c r="Y31">
+        <f t="shared" si="3"/>
+        <v>34.269145281217334</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -11158,11 +11259,15 @@
         <v>27.855414794546121</v>
       </c>
       <c r="X32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.865092253138137</v>
       </c>
+      <c r="Y32">
+        <f t="shared" si="3"/>
+        <v>30.053353159364317</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -11230,11 +11335,193 @@
         <v>60.616973137270598</v>
       </c>
       <c r="X33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1839339568322087</v>
       </c>
+      <c r="Y33">
+        <f t="shared" si="3"/>
+        <v>60.617398611085314</v>
+      </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <f>_xlfn.STDEV.S(B30:B33)</f>
+        <v>35.416905582382263</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:V35" si="4">_xlfn.STDEV.S(C30:C33)</f>
+        <v>15.68654183375452</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>19.899139858945329</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>17.433802622092692</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>18.723234923958739</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>16.976752855914054</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>19.104292121682747</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>18.2728683619907</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>19.589320143579414</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>17.075883324551317</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="4"/>
+        <v>14.87598634674664</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="4"/>
+        <v>17.679519453555415</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>15.970168933263425</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="4"/>
+        <v>17.718576801147726</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>14.638925589392452</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="4"/>
+        <v>14.91533337130876</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="4"/>
+        <v>15.910160448501927</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="4"/>
+        <v>12.769598492132964</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="4"/>
+        <v>17.078808481834148</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="4"/>
+        <v>13.56369333549403</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="4"/>
+        <v>16.408510078695411</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <f>AVERAGE(B30:B33)</f>
+        <v>106.01982889118253</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:V36" si="5">AVERAGE(C30:C33)</f>
+        <v>45.905575671212347</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>37.523621183883861</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="5"/>
+        <v>40.252853958558248</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="5"/>
+        <v>38.97962598299798</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>36.198320211088657</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="5"/>
+        <v>38.771936057086549</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>39.802860327206254</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>37.64717013485479</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>34.607583617520014</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="5"/>
+        <v>42.33029628838576</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>37.815640222881186</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>37.265313481358469</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="5"/>
+        <v>36.07392244238082</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="5"/>
+        <v>35.334521458841635</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>34.839361673219599</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="5"/>
+        <v>35.701102276036913</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="5"/>
+        <v>41.827679246792542</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>38.662033978452861</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="5"/>
+        <v>33.191746332220127</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="5"/>
+        <v>36.018632864588895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -11242,7 +11529,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -11312,8 +11599,11 @@
       <c r="X43" t="s">
         <v>36</v>
       </c>
+      <c r="Y43" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -11381,11 +11671,15 @@
         <v>88.256337246149229</v>
       </c>
       <c r="X44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.371720861967592</v>
       </c>
+      <c r="Y44">
+        <f t="shared" ref="Y44:Y51" si="6">AVERAGE(,B44:V44)</f>
+        <v>93.427221468920209</v>
+      </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -11453,11 +11747,15 @@
         <v>94.668206109532861</v>
       </c>
       <c r="X45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.519656818402783</v>
       </c>
+      <c r="Y45">
+        <f t="shared" si="6"/>
+        <v>96.413664668044518</v>
+      </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -11525,11 +11823,15 @@
         <v>77.876428589112265</v>
       </c>
       <c r="X46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.766626895184523</v>
       </c>
+      <c r="Y46">
+        <f t="shared" si="6"/>
+        <v>88.160899139978994</v>
+      </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -11597,11 +11899,15 @@
         <v>99.075491960290421</v>
       </c>
       <c r="X47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.412305813036735</v>
       </c>
+      <c r="Y47">
+        <f t="shared" si="6"/>
+        <v>99.505405980760131</v>
+      </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>29</v>
       </c>
@@ -11669,11 +11975,15 @@
         <v>91.528346754051896</v>
       </c>
       <c r="X48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.528180146411751</v>
       </c>
+      <c r="Y48">
+        <f t="shared" si="6"/>
+        <v>96.711062594147634</v>
+      </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>30</v>
       </c>
@@ -11741,11 +12051,15 @@
         <v>100.7087499765652</v>
       </c>
       <c r="X49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.906094774627583</v>
       </c>
+      <c r="Y49">
+        <f t="shared" si="6"/>
+        <v>100.24853968275418</v>
+      </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>31</v>
       </c>
@@ -11813,11 +12127,15 @@
         <v>89.261928464203805</v>
       </c>
       <c r="X50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.812826027300964</v>
       </c>
+      <c r="Y50">
+        <f t="shared" si="6"/>
+        <v>96.855349662956002</v>
+      </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>32</v>
       </c>
@@ -11885,11 +12203,15 @@
         <v>94.982865587684756</v>
       </c>
       <c r="X51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.309520167265561</v>
       </c>
+      <c r="Y51">
+        <f t="shared" si="6"/>
+        <v>92.995386692709019</v>
+      </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -11897,7 +12219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -11967,8 +12289,11 @@
       <c r="X57" t="s">
         <v>36</v>
       </c>
+      <c r="Y57" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>22</v>
       </c>
@@ -12036,11 +12361,15 @@
         <v>31.00095724184218</v>
       </c>
       <c r="X58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8848921172493549</v>
       </c>
+      <c r="Y58">
+        <f t="shared" ref="Y58:Y61" si="7">AVERAGE(,B58:V58)</f>
+        <v>32.616585256338375</v>
+      </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>23</v>
       </c>
@@ -12108,11 +12437,15 @@
         <v>29.14481129774072</v>
       </c>
       <c r="X59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4953612489459811</v>
       </c>
+      <c r="Y59">
+        <f t="shared" si="7"/>
+        <v>34.095295466948819</v>
+      </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
@@ -12180,11 +12513,15 @@
         <v>35.272670649656121</v>
       </c>
       <c r="X60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0258684516713332</v>
       </c>
+      <c r="Y60">
+        <f t="shared" si="7"/>
+        <v>34.366061754448189</v>
+      </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
@@ -12252,11 +12589,15 @@
         <v>59.597435433371103</v>
       </c>
       <c r="X61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3823925227010454</v>
       </c>
+      <c r="Y61">
+        <f t="shared" si="7"/>
+        <v>61.257713818928487</v>
+      </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -12264,7 +12605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -12334,8 +12675,11 @@
       <c r="X71" t="s">
         <v>36</v>
       </c>
+      <c r="Y71" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>22</v>
       </c>
@@ -12403,11 +12747,15 @@
         <v>102.9549449709008</v>
       </c>
       <c r="X72">
-        <f t="shared" ref="X69:X108" si="1">_xlfn.STDEV.S(B72:V72)</f>
+        <f t="shared" ref="X72:X108" si="8">_xlfn.STDEV.S(B72:V72)</f>
         <v>33.45672602369357</v>
       </c>
+      <c r="Y72">
+        <f t="shared" ref="Y72:Y79" si="9">AVERAGE(,B72:V72)</f>
+        <v>124.3051504514072</v>
+      </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>23</v>
       </c>
@@ -12475,11 +12823,15 @@
         <v>102.17849213139471</v>
       </c>
       <c r="X73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>29.772224437426797</v>
       </c>
+      <c r="Y73">
+        <f t="shared" si="9"/>
+        <v>121.75682592405479</v>
+      </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -12547,11 +12899,15 @@
         <v>103.90092210631509</v>
       </c>
       <c r="X74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>20.108183841087783</v>
       </c>
+      <c r="Y74">
+        <f t="shared" si="9"/>
+        <v>112.55833545664919</v>
+      </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>25</v>
       </c>
@@ -12619,11 +12975,15 @@
         <v>102.5202229226483</v>
       </c>
       <c r="X75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>28.694700435111905</v>
       </c>
+      <c r="Y75">
+        <f t="shared" si="9"/>
+        <v>117.06005636207543</v>
+      </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>29</v>
       </c>
@@ -12691,11 +13051,15 @@
         <v>105.6004951490667</v>
       </c>
       <c r="X76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>30.805826702161582</v>
       </c>
+      <c r="Y76">
+        <f t="shared" si="9"/>
+        <v>117.09968965332854</v>
+      </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>30</v>
       </c>
@@ -12763,11 +13127,15 @@
         <v>102.2291343548668</v>
       </c>
       <c r="X77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>30.196161187343197</v>
       </c>
+      <c r="Y77">
+        <f t="shared" si="9"/>
+        <v>120.07061499641712</v>
+      </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>31</v>
       </c>
@@ -12835,11 +13203,15 @@
         <v>102.6122275032883</v>
       </c>
       <c r="X78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>33.196783229334102</v>
       </c>
+      <c r="Y78">
+        <f t="shared" si="9"/>
+        <v>118.8548925914134</v>
+      </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>32</v>
       </c>
@@ -12907,11 +13279,15 @@
         <v>104.1084006734318</v>
       </c>
       <c r="X79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>33.429205432392081</v>
       </c>
+      <c r="Y79">
+        <f t="shared" si="9"/>
+        <v>122.73214697367358</v>
+      </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>35</v>
       </c>
@@ -12919,7 +13295,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -12989,8 +13365,11 @@
       <c r="X86" t="s">
         <v>36</v>
       </c>
+      <c r="Y86" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>22</v>
       </c>
@@ -13058,11 +13437,15 @@
         <v>31.285886825121828</v>
       </c>
       <c r="X87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>8.6538329472599749</v>
       </c>
+      <c r="Y87">
+        <f t="shared" ref="Y87:Y94" si="10">AVERAGE(,B87:V87)</f>
+        <v>30.952416991408413</v>
+      </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>23</v>
       </c>
@@ -13130,11 +13513,15 @@
         <v>29.588661309927168</v>
       </c>
       <c r="X88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>9.0514906295733297</v>
       </c>
+      <c r="Y88">
+        <f t="shared" si="10"/>
+        <v>30.362306751522592</v>
+      </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -13202,11 +13589,15 @@
         <v>29.72674764903606</v>
       </c>
       <c r="X89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>8.3073613469965242</v>
       </c>
+      <c r="Y89">
+        <f t="shared" si="10"/>
+        <v>30.299180821565471</v>
+      </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>25</v>
       </c>
@@ -13274,11 +13665,15 @@
         <v>59.127778620768353</v>
       </c>
       <c r="X90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>4.4431520726369245</v>
       </c>
+      <c r="Y90">
+        <f t="shared" si="10"/>
+        <v>59.364771474602911</v>
+      </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -13286,7 +13681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -13353,8 +13748,14 @@
       <c r="V100" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="X100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y100" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
         <v>22</v>
       </c>
@@ -13422,11 +13823,15 @@
         <v>127.4170902111468</v>
       </c>
       <c r="X101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>19.066348041212631</v>
       </c>
+      <c r="Y101">
+        <f t="shared" ref="Y101:Y108" si="11">AVERAGE(,B101:V101)</f>
+        <v>133.06920758784466</v>
+      </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
         <v>23</v>
       </c>
@@ -13494,11 +13899,15 @@
         <v>129.52915227342291</v>
       </c>
       <c r="X102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>26.484598857505954</v>
       </c>
+      <c r="Y102">
+        <f t="shared" si="11"/>
+        <v>128.00402676664106</v>
+      </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
         <v>24</v>
       </c>
@@ -13566,11 +13975,15 @@
         <v>128.6300225489228</v>
       </c>
       <c r="X103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>19.874753646557402</v>
       </c>
+      <c r="Y103">
+        <f t="shared" si="11"/>
+        <v>127.05683401827601</v>
+      </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
         <v>25</v>
       </c>
@@ -13638,11 +14051,15 @@
         <v>122.0265930366762</v>
       </c>
       <c r="X104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>19.709267895731376</v>
       </c>
+      <c r="Y104">
+        <f t="shared" si="11"/>
+        <v>127.59176266395519</v>
+      </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
         <v>29</v>
       </c>
@@ -13710,11 +14127,15 @@
         <v>119.9198000183781</v>
       </c>
       <c r="X105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>20.330001057546795</v>
       </c>
+      <c r="Y105">
+        <f t="shared" si="11"/>
+        <v>130.6067720069897</v>
+      </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
         <v>30</v>
       </c>
@@ -13782,11 +14203,15 @@
         <v>127.27274977422471</v>
       </c>
       <c r="X106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>22.294577502528078</v>
       </c>
+      <c r="Y106">
+        <f t="shared" si="11"/>
+        <v>125.11652361527091</v>
+      </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
         <v>31</v>
       </c>
@@ -13854,11 +14279,15 @@
         <v>122.40546579647</v>
       </c>
       <c r="X107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>21.90246106072405</v>
       </c>
+      <c r="Y107">
+        <f t="shared" si="11"/>
+        <v>129.98874662863946</v>
+      </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
         <v>32</v>
       </c>
@@ -13926,13 +14355,18 @@
         <v>138.85456296044671</v>
       </c>
       <c r="X108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>18.422765898177563</v>
+      </c>
+      <c r="Y108">
+        <f t="shared" si="11"/>
+        <v>133.60079576179069</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>